<commit_message>
tumor type mapping errors
</commit_message>
<xml_diff>
--- a/data/source/pedpancan_mapping.xlsx
+++ b/data/source/pedpancan_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkenkre/Desktop/pedpancancer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ochapman/projects/pedpancan_ecdna/data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C5A365-7866-7F40-96A9-058785B087EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F657600F-D32C-604C-93A3-B9737DA41E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1560" windowWidth="20080" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mapping" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1620" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1673" uniqueCount="369">
   <si>
     <t>Column</t>
   </si>
@@ -1045,13 +1045,97 @@
   </si>
   <si>
     <t>TALLNOS</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>I have no idea where to put a CNS_BCOR_ITD (CNS tumor, BCOR internal tandem dup) but I don't see justification for calling it a DNET</t>
+  </si>
+  <si>
+    <t>*1 Combine GM and TT into a GCT class?</t>
+  </si>
+  <si>
+    <t>*1</t>
+  </si>
+  <si>
+    <t>Should be SEGA?</t>
+  </si>
+  <si>
+    <t>Should be GNT?</t>
+  </si>
+  <si>
+    <t>No idea what to do with a PLNTY (polymorphous low grade brain tumor of the young) but I don't see any connection with meningioma</t>
+  </si>
+  <si>
+    <t>BTNOS?</t>
+  </si>
+  <si>
+    <t>Should be CPG?</t>
+  </si>
+  <si>
+    <t>We already have a MG class for meningioma. Although, I think MNG would be better than MG because nature disapproves of 2-letter abbreviations.</t>
+  </si>
+  <si>
+    <t>Should be GCT?</t>
+  </si>
+  <si>
+    <t>Glioma, not otherwise specified. Not specific enough to call it a ganglioglioma.</t>
+  </si>
+  <si>
+    <t>Should be DNET? Also, this is a duplicate entry of DNT -&gt; DNET above.</t>
+  </si>
+  <si>
+    <t>Should be GNT? Also duplicate of LGGNT &gt; GG above.</t>
+  </si>
+  <si>
+    <t>Should be NBL?</t>
+  </si>
+  <si>
+    <t>Shouldn be CRD?</t>
+  </si>
+  <si>
+    <t>Should be RHB?</t>
+  </si>
+  <si>
+    <t>Should Be NFP?</t>
+  </si>
+  <si>
+    <t>Duplicate of WTB &gt; WLM below</t>
+  </si>
+  <si>
+    <t>*2 Since we don't discuss hematopoetic malignancies, I think we should lump all blood cancers into a HM group</t>
+  </si>
+  <si>
+    <t>Duplicate of ACC &gt; ACT above</t>
+  </si>
+  <si>
+    <t>Why rename it?</t>
+  </si>
+  <si>
+    <t>Duplicate of EWS &gt; EWS above</t>
+  </si>
+  <si>
+    <t>*2</t>
+  </si>
+  <si>
+    <t>*3 We discussed moving on to the next priority order if we encounter a control sample</t>
+  </si>
+  <si>
+    <t>All other astrocytomas are being classed as HGG or LGG, but no idea which one this should go to.</t>
+  </si>
+  <si>
+    <t>*3</t>
+  </si>
+  <si>
+    <t>We already have an EP class for ependymoma. But I like EPN better, see the MG/MNG comment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1193,8 +1277,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1392,6 +1482,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1553,14 +1649,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1919,7 +2017,7 @@
   <dimension ref="A1:C172"/>
   <sheetViews>
     <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:XFD98"/>
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3827,20 +3925,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C305"/>
+  <dimension ref="A1:D305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="B147" sqref="B147"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="2" max="2" width="72.83203125" customWidth="1"/>
-    <col min="3" max="3" width="78.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3850,8 +3949,11 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -3862,7 +3964,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -3873,7 +3975,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -3884,7 +3986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -3895,7 +3997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -3906,7 +4008,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -3917,7 +4019,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -3928,7 +4030,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -3939,7 +4041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -3950,7 +4052,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -3961,7 +4063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -3972,7 +4074,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
@@ -3983,7 +4085,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
@@ -3994,7 +4096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -4005,7 +4107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>12</v>
       </c>
@@ -4016,7 +4118,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
@@ -4027,7 +4129,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
@@ -4038,7 +4140,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>3</v>
       </c>
@@ -4049,7 +4151,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
@@ -4060,7 +4162,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>29</v>
       </c>
@@ -4071,7 +4173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>9</v>
       </c>
@@ -4082,7 +4184,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>9</v>
       </c>
@@ -4093,7 +4195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
@@ -4104,7 +4206,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>12</v>
       </c>
@@ -4115,7 +4217,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>3</v>
       </c>
@@ -4126,7 +4228,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>3</v>
       </c>
@@ -4137,7 +4239,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>12</v>
       </c>
@@ -4148,7 +4250,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>12</v>
       </c>
@@ -4159,7 +4261,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>12</v>
       </c>
@@ -4170,7 +4272,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>12</v>
       </c>
@@ -4181,7 +4283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>9</v>
       </c>
@@ -4192,7 +4294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>12</v>
       </c>
@@ -4203,18 +4305,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>3</v>
       </c>
@@ -4225,7 +4330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>3</v>
       </c>
@@ -4236,7 +4341,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>3</v>
       </c>
@@ -4247,7 +4352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>3</v>
       </c>
@@ -4258,7 +4363,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>3</v>
       </c>
@@ -4269,7 +4374,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
@@ -4280,7 +4385,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>3</v>
       </c>
@@ -4291,7 +4396,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>3</v>
       </c>
@@ -4302,7 +4407,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>3</v>
       </c>
@@ -4313,7 +4418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>9</v>
       </c>
@@ -4324,7 +4429,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>3</v>
       </c>
@@ -4335,7 +4440,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>3</v>
       </c>
@@ -4346,7 +4451,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>3</v>
       </c>
@@ -4357,7 +4462,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>3</v>
       </c>
@@ -4368,7 +4473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>3</v>
       </c>
@@ -4379,7 +4484,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>3</v>
       </c>
@@ -4390,7 +4495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>3</v>
       </c>
@@ -4401,7 +4506,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>3</v>
       </c>
@@ -4412,7 +4517,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>3</v>
       </c>
@@ -4423,7 +4528,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>3</v>
       </c>
@@ -4434,7 +4539,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>3</v>
       </c>
@@ -4445,7 +4550,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>3</v>
       </c>
@@ -4456,7 +4561,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>3</v>
       </c>
@@ -4467,7 +4572,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>3</v>
       </c>
@@ -4478,7 +4583,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>3</v>
       </c>
@@ -4489,7 +4594,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>3</v>
       </c>
@@ -4500,29 +4605,35 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
+      <c r="D61" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>9</v>
       </c>
@@ -4533,7 +4644,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>12</v>
       </c>
@@ -4544,7 +4655,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>3</v>
       </c>
@@ -4555,7 +4666,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>3</v>
       </c>
@@ -4566,7 +4677,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>3</v>
       </c>
@@ -4577,7 +4688,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>3</v>
       </c>
@@ -4588,7 +4699,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>3</v>
       </c>
@@ -4599,7 +4710,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>3</v>
       </c>
@@ -4610,7 +4721,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>3</v>
       </c>
@@ -4621,7 +4732,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>3</v>
       </c>
@@ -4632,7 +4743,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>3</v>
       </c>
@@ -4643,7 +4754,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>3</v>
       </c>
@@ -4654,7 +4765,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>3</v>
       </c>
@@ -4665,7 +4776,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>3</v>
       </c>
@@ -4676,7 +4787,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>3</v>
       </c>
@@ -4687,7 +4798,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>3</v>
       </c>
@@ -4698,7 +4809,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>3</v>
       </c>
@@ -4709,7 +4820,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>3</v>
       </c>
@@ -4720,7 +4831,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>3</v>
       </c>
@@ -4731,7 +4842,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>3</v>
       </c>
@@ -4742,7 +4853,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>3</v>
       </c>
@@ -4753,7 +4864,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>3</v>
       </c>
@@ -4764,7 +4875,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>29</v>
       </c>
@@ -4775,7 +4886,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>29</v>
       </c>
@@ -4786,7 +4897,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>9</v>
       </c>
@@ -4797,7 +4908,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>12</v>
       </c>
@@ -4808,7 +4919,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>3</v>
       </c>
@@ -4819,7 +4930,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>3</v>
       </c>
@@ -4830,7 +4941,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>3</v>
       </c>
@@ -4841,7 +4952,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>3</v>
       </c>
@@ -4852,7 +4963,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>3</v>
       </c>
@@ -4863,7 +4974,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>3</v>
       </c>
@@ -4874,7 +4985,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>3</v>
       </c>
@@ -4885,7 +4996,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>3</v>
       </c>
@@ -4896,7 +5007,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>3</v>
       </c>
@@ -4907,7 +5018,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>3</v>
       </c>
@@ -4918,7 +5029,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>3</v>
       </c>
@@ -4929,7 +5040,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>3</v>
       </c>
@@ -4940,7 +5051,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>3</v>
       </c>
@@ -4951,7 +5062,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>3</v>
       </c>
@@ -4962,7 +5073,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>3</v>
       </c>
@@ -4973,7 +5084,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>3</v>
       </c>
@@ -4984,7 +5095,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>3</v>
       </c>
@@ -4995,7 +5106,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>3</v>
       </c>
@@ -5006,7 +5117,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>3</v>
       </c>
@@ -5017,7 +5128,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>3</v>
       </c>
@@ -5028,7 +5139,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>3</v>
       </c>
@@ -5039,18 +5150,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B110" s="4" t="s">
+    <row r="110" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D110" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>3</v>
       </c>
@@ -5061,7 +5175,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>3</v>
       </c>
@@ -5072,18 +5186,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B113" s="4" t="s">
+    <row r="113" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B113" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C113" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D113" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>3</v>
       </c>
@@ -5094,7 +5211,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>3</v>
       </c>
@@ -5105,18 +5222,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B116" s="4" t="s">
+    <row r="116" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D116" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>3</v>
       </c>
@@ -5127,7 +5247,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>3</v>
       </c>
@@ -5138,7 +5258,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>3</v>
       </c>
@@ -5149,7 +5269,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>3</v>
       </c>
@@ -5160,7 +5280,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>3</v>
       </c>
@@ -5171,7 +5291,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>9</v>
       </c>
@@ -5182,7 +5302,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>35</v>
       </c>
@@ -5193,7 +5313,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>9</v>
       </c>
@@ -5204,7 +5324,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>9</v>
       </c>
@@ -5215,7 +5335,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>12</v>
       </c>
@@ -5226,7 +5346,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>12</v>
       </c>
@@ -5237,7 +5357,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>9</v>
       </c>
@@ -5248,7 +5368,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>9</v>
       </c>
@@ -5259,7 +5379,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>9</v>
       </c>
@@ -5270,18 +5390,21 @@
         <v>165</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+    <row r="131" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C131" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D131" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>12</v>
       </c>
@@ -5292,7 +5415,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>12</v>
       </c>
@@ -5303,7 +5426,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>9</v>
       </c>
@@ -5314,7 +5437,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>12</v>
       </c>
@@ -5325,7 +5448,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>9</v>
       </c>
@@ -5336,7 +5459,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>9</v>
       </c>
@@ -5347,7 +5470,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>12</v>
       </c>
@@ -5358,7 +5481,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>3</v>
       </c>
@@ -5369,7 +5492,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>3</v>
       </c>
@@ -5380,7 +5503,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>3</v>
       </c>
@@ -5391,7 +5514,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>12</v>
       </c>
@@ -5402,7 +5525,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>9</v>
       </c>
@@ -5413,7 +5536,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>12</v>
       </c>
@@ -5424,7 +5547,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>9</v>
       </c>
@@ -5435,7 +5558,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
         <v>12</v>
       </c>
@@ -5446,7 +5569,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
         <v>9</v>
       </c>
@@ -5457,7 +5580,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
         <v>12</v>
       </c>
@@ -5468,7 +5591,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149" s="4" t="s">
         <v>9</v>
       </c>
@@ -5479,7 +5602,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
         <v>12</v>
       </c>
@@ -5490,7 +5613,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151" s="4" t="s">
         <v>12</v>
       </c>
@@ -5501,7 +5624,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
         <v>3</v>
       </c>
@@ -5512,228 +5635,258 @@
         <v>207</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" s="4" t="s">
+    <row r="153" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B153" s="4" t="s">
+      <c r="B153" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C153" s="4" t="s">
+      <c r="C153" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="4" t="s">
+      <c r="D153" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B154" s="4" t="s">
+      <c r="B154" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C154" s="4" t="s">
+      <c r="C154" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" s="4" t="s">
+      <c r="D154" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B155" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C155" s="4" t="s">
+      <c r="C155" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D155" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B156" s="6" t="s">
+      <c r="B156" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C156" s="6" t="s">
+      <c r="C156" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B157" s="6" t="s">
+      <c r="D156" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" t="s">
         <v>219</v>
       </c>
-      <c r="C157" s="6" t="s">
+      <c r="C157" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="158" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A158" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B158" s="6" t="s">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B158" t="s">
         <v>230</v>
       </c>
-      <c r="C158" s="6" t="s">
+      <c r="C158" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="159" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B159" s="6" t="s">
+      <c r="B159" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="C159" s="6" t="s">
+      <c r="C159" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D159" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B160" s="6" t="s">
+      <c r="B160" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C160" s="6" t="s">
+      <c r="C160" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D160" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B161" s="6" t="s">
+      <c r="B161" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C161" s="6" t="s">
+      <c r="C161" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B162" s="6" t="s">
+      <c r="D161" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B162" t="s">
         <v>233</v>
       </c>
-      <c r="C162" s="6" t="s">
+      <c r="C162" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B163" s="6" t="s">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B163" t="s">
         <v>234</v>
       </c>
-      <c r="C163" s="6" t="s">
+      <c r="C163" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="164" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B164" s="6" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B164" t="s">
         <v>235</v>
       </c>
-      <c r="C164" s="6" t="s">
+      <c r="C164" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="165" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B165" s="6" t="s">
+      <c r="B165" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C165" s="6" t="s">
+      <c r="C165" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B166" s="6" t="s">
+      <c r="D165" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B166" t="s">
         <v>5</v>
       </c>
-      <c r="C166" s="6" t="s">
+      <c r="C166" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B167" s="6" t="s">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B167" t="s">
         <v>237</v>
       </c>
-      <c r="C167" s="6" t="s">
+      <c r="C167" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="168" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B168" s="6" t="s">
+      <c r="B168" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C168" s="6" t="s">
+      <c r="C168" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D168" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B169" s="6" t="s">
+      <c r="B169" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C169" s="6" t="s">
+      <c r="C169" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B170" s="6" t="s">
+      <c r="D169" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B170" t="s">
         <v>240</v>
       </c>
-      <c r="C170" s="6" t="s">
+      <c r="C170" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="171" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B171" s="6" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B171" t="s">
         <v>241</v>
       </c>
-      <c r="C171" s="6" t="s">
+      <c r="C171" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="172" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B172" s="6" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B172" t="s">
         <v>242</v>
       </c>
-      <c r="C172" s="6" t="s">
+      <c r="C172" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A173" s="5" t="s">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="7" t="s">
         <v>312</v>
       </c>
       <c r="B173" s="6" t="s">
@@ -5743,1385 +5896,1454 @@
         <v>311</v>
       </c>
     </row>
-    <row r="174" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B174" s="6" t="s">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B174" t="s">
         <v>70</v>
       </c>
-      <c r="C174" s="6" t="s">
+      <c r="C174" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="175" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B175" s="6" t="s">
+      <c r="B175" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C175" s="6" t="s">
+      <c r="C175" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B176" s="6" t="s">
+      <c r="D175" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B176" t="s">
         <v>245</v>
       </c>
-      <c r="C176" s="6" t="s">
+      <c r="C176" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="177" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B177" s="6" t="s">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B177" t="s">
         <v>25</v>
       </c>
-      <c r="C177" s="6" t="s">
+      <c r="C177" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="178" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B178" s="6" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B178" t="s">
         <v>220</v>
       </c>
-      <c r="C178" s="6" t="s">
+      <c r="C178" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="179" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A179" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B179" s="6" t="s">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B179" t="s">
         <v>246</v>
       </c>
-      <c r="C179" s="6" t="s">
+      <c r="C179" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="180" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A180" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B180" s="6" t="s">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B180" t="s">
         <v>72</v>
       </c>
-      <c r="C180" s="6" t="s">
+      <c r="C180" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="181" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B181" s="6" t="s">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B181" t="s">
         <v>222</v>
       </c>
-      <c r="C181" s="6" t="s">
+      <c r="C181" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="182" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A182" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B182" s="6" t="s">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B182" t="s">
         <v>230</v>
       </c>
-      <c r="C182" s="6" t="s">
+      <c r="C182" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="183" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A183" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B183" s="6" t="s">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B183" t="s">
         <v>70</v>
       </c>
-      <c r="C183" s="6" t="s">
+      <c r="C183" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="184" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A184" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B184" s="6" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B184" t="s">
         <v>233</v>
       </c>
-      <c r="C184" s="6" t="s">
+      <c r="C184" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="185" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B185" s="6" t="s">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B185" t="s">
         <v>247</v>
       </c>
-      <c r="C185" s="6" t="s">
+      <c r="C185" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="186" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B186" s="6" t="s">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B186" t="s">
         <v>248</v>
       </c>
-      <c r="C186" s="6" t="s">
+      <c r="C186" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="187" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B187" s="6" t="s">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B187" t="s">
         <v>249</v>
       </c>
-      <c r="C187" s="6" t="s">
+      <c r="C187" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="188" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B188" s="6" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B188" t="s">
         <v>250</v>
       </c>
-      <c r="C188" s="6" t="s">
+      <c r="C188" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="189" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B189" s="6" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B189" t="s">
         <v>251</v>
       </c>
-      <c r="C189" s="6" t="s">
+      <c r="C189" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="190" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B190" s="6" t="s">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B190" t="s">
         <v>252</v>
       </c>
-      <c r="C190" s="6" t="s">
+      <c r="C190" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="191" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B191" s="6" t="s">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B191" t="s">
         <v>253</v>
       </c>
-      <c r="C191" s="6" t="s">
+      <c r="C191" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="192" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B192" s="6" t="s">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B192" t="s">
         <v>254</v>
       </c>
-      <c r="C192" s="6" t="s">
+      <c r="C192" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="193" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A193" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B193" s="6" t="s">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B193" t="s">
         <v>255</v>
       </c>
-      <c r="C193" s="6" t="s">
+      <c r="C193" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="194" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B194" s="6" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B194" t="s">
         <v>256</v>
       </c>
-      <c r="C194" s="6" t="s">
+      <c r="C194" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="195" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A195" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B195" s="6" t="s">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B195" t="s">
         <v>257</v>
       </c>
-      <c r="C195" s="6" t="s">
+      <c r="C195" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="196" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A196" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B196" s="6" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B196" t="s">
         <v>258</v>
       </c>
-      <c r="C196" s="6" t="s">
+      <c r="C196" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="197" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A197" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B197" s="6" t="s">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B197" t="s">
         <v>223</v>
       </c>
-      <c r="C197" s="6" t="s">
+      <c r="C197" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="198" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A198" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B198" s="6" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B198" t="s">
         <v>259</v>
       </c>
-      <c r="C198" s="6" t="s">
+      <c r="C198" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="199" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B199" s="6" t="s">
+      <c r="B199" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C199" s="6" t="s">
+      <c r="C199" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D199" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B200" s="6" t="s">
+      <c r="B200" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C200" s="6" t="s">
+      <c r="C200" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A201" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B201" s="6" t="s">
+      <c r="D200" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B201" t="s">
         <v>213</v>
       </c>
-      <c r="C201" s="6" t="s">
+      <c r="C201" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="202" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B202" s="6" t="s">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B202" t="s">
         <v>260</v>
       </c>
-      <c r="C202" s="6" t="s">
+      <c r="C202" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B203" s="6" t="s">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B203" t="s">
         <v>176</v>
       </c>
-      <c r="C203" s="6" t="s">
+      <c r="C203" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="204" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B204" s="6" t="s">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B204" t="s">
         <v>182</v>
       </c>
-      <c r="C204" s="6" t="s">
+      <c r="C204" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="205" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B205" s="6" t="s">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B205" t="s">
         <v>95</v>
       </c>
-      <c r="C205" s="6" t="s">
+      <c r="C205" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="206" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B206" s="6" t="s">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B206" t="s">
         <v>214</v>
       </c>
-      <c r="C206" s="6" t="s">
+      <c r="C206" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="207" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B207" s="6" t="s">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B207" t="s">
         <v>261</v>
       </c>
-      <c r="C207" s="6" t="s">
+      <c r="C207" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="208" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A208" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B208" s="6" t="s">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B208" t="s">
         <v>262</v>
       </c>
-      <c r="C208" s="6" t="s">
+      <c r="C208" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="209" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B209" s="6" t="s">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B209" t="s">
         <v>263</v>
       </c>
-      <c r="C209" s="6" t="s">
+      <c r="C209" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="210" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A210" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B210" s="6" t="s">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B210" t="s">
         <v>264</v>
       </c>
-      <c r="C210" s="6" t="s">
+      <c r="C210" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="211" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B211" s="6" t="s">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B211" t="s">
         <v>201</v>
       </c>
-      <c r="C211" s="6" t="s">
+      <c r="C211" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="212" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B212" s="6" t="s">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B212" t="s">
         <v>202</v>
       </c>
-      <c r="C212" s="6" t="s">
+      <c r="C212" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="213" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A213" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B213" s="6" t="s">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B213" t="s">
         <v>265</v>
       </c>
-      <c r="C213" s="6" t="s">
+      <c r="C213" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="214" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A214" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B214" s="6" t="s">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B214" t="s">
         <v>266</v>
       </c>
-      <c r="C214" s="6" t="s">
+      <c r="C214" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="215" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A215" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B215" s="6" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B215" t="s">
         <v>267</v>
       </c>
-      <c r="C215" s="6" t="s">
+      <c r="C215" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="216" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B216" s="6" t="s">
+      <c r="B216" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C216" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B217" s="6" t="s">
+      <c r="C216" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B217" t="s">
         <v>268</v>
       </c>
-      <c r="C217" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B218" s="6" t="s">
+      <c r="C217" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B218" t="s">
         <v>269</v>
       </c>
-      <c r="C218" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B219" s="6" t="s">
+      <c r="C218" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B219" t="s">
         <v>270</v>
       </c>
-      <c r="C219" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B220" s="6" t="s">
+      <c r="C219" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B220" t="s">
         <v>271</v>
       </c>
-      <c r="C220" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A221" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B221" s="6" t="s">
+      <c r="C220" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B221" t="s">
         <v>272</v>
       </c>
-      <c r="C221" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A222" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B222" s="6" t="s">
+      <c r="C221" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B222" t="s">
         <v>273</v>
       </c>
-      <c r="C222" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A223" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B223" s="6" t="s">
+      <c r="C222" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B223" t="s">
         <v>274</v>
       </c>
-      <c r="C223" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B224" s="6" t="s">
+      <c r="C223" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B224" t="s">
         <v>275</v>
       </c>
-      <c r="C224" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B225" s="6" t="s">
+      <c r="C224" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B225" t="s">
         <v>276</v>
       </c>
-      <c r="C225" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C225" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B226" s="6" t="s">
+      <c r="B226" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="C226" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A227" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B227" s="6" t="s">
+      <c r="C226" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B227" t="s">
         <v>278</v>
       </c>
-      <c r="C227" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C227" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B228" s="6" t="s">
+      <c r="B228" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C228" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C228" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D228" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B229" s="6" t="s">
+      <c r="B229" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="C229" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A230" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B230" s="6" t="s">
+      <c r="C229" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D229" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B230" t="s">
         <v>280</v>
       </c>
-      <c r="C230" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A231" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B231" s="6" t="s">
+      <c r="C230" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B231" t="s">
         <v>281</v>
       </c>
-      <c r="C231" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A232" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B232" s="6" t="s">
+      <c r="C231" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B232" t="s">
         <v>282</v>
       </c>
-      <c r="C232" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A233" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B233" s="6" t="s">
+      <c r="C232" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B233" t="s">
         <v>229</v>
       </c>
-      <c r="C233" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B234" s="6" t="s">
+      <c r="C233" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B234" t="s">
         <v>283</v>
       </c>
-      <c r="C234" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A235" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B235" s="6" t="s">
+      <c r="C234" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B235" t="s">
         <v>284</v>
       </c>
-      <c r="C235" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B236" s="6" t="s">
+      <c r="C235" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B236" t="s">
         <v>285</v>
       </c>
-      <c r="C236" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C236" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A237" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B237" s="6" t="s">
+      <c r="B237" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="C237" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C237" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B238" s="6" t="s">
+      <c r="B238" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C238" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A239" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B239" s="6" t="s">
+      <c r="C238" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D238" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B239" t="s">
         <v>288</v>
       </c>
-      <c r="C239" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C239" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A240" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B240" s="6" t="s">
+      <c r="B240" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="C240" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A241" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B241" s="6" t="s">
+      <c r="C240" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B241" t="s">
         <v>290</v>
       </c>
-      <c r="C241" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A242" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B242" s="6" t="s">
+      <c r="C241" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B242" t="s">
         <v>291</v>
       </c>
-      <c r="C242" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C242" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B243" s="6" t="s">
+      <c r="B243" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C243" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C243" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A244" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B244" s="6" t="s">
+      <c r="B244" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C244" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="245" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A245" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B245" s="6" t="s">
+      <c r="C244" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D244" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B245" t="s">
         <v>293</v>
       </c>
-      <c r="C245" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="246" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C245" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A246" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B246" s="6" t="s">
+      <c r="B246" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C246" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C246" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B247" s="6" t="s">
+      <c r="B247" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C247" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A248" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B248" s="6" t="s">
+      <c r="C247" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B248" t="s">
         <v>294</v>
       </c>
-      <c r="C248" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C248" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B249" s="6" t="s">
+      <c r="B249" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C249" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C249" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A250" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B250" s="6" t="s">
+      <c r="B250" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C250" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A251" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B251" s="6" t="s">
+      <c r="C250" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B251" t="s">
         <v>296</v>
       </c>
-      <c r="C251" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A252" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B252" s="6" t="s">
+      <c r="C251" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A252" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B252" t="s">
         <v>297</v>
       </c>
-      <c r="C252" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A253" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B253" s="6" t="s">
+      <c r="C252" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A253" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B253" t="s">
         <v>298</v>
       </c>
-      <c r="C253" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A254" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B254" s="6" t="s">
+      <c r="C253" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A254" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B254" t="s">
         <v>299</v>
       </c>
-      <c r="C254" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A255" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B255" s="6" t="s">
+      <c r="C254" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A255" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B255" t="s">
         <v>300</v>
       </c>
-      <c r="C255" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A256" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B256" s="6" t="s">
+      <c r="C255" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A256" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B256" t="s">
         <v>301</v>
       </c>
-      <c r="C256" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C256" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B257" s="6" t="s">
+      <c r="B257" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C257" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A258" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B258" s="6" t="s">
+      <c r="C257" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D257" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A258" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B258" t="s">
         <v>267</v>
       </c>
-      <c r="C258" s="6" t="s">
+      <c r="C258" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="259" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A259" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B259" s="6" t="s">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A259" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B259" t="s">
         <v>292</v>
       </c>
-      <c r="C259" s="6" t="s">
+      <c r="C259" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="260" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A260" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B260" s="6" t="s">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A260" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B260" t="s">
         <v>302</v>
       </c>
-      <c r="C260" s="6" t="s">
+      <c r="C260" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="261" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B261" s="6" t="s">
+      <c r="B261" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C261" s="6" t="s">
+      <c r="C261" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="262" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A262" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B262" s="6" t="s">
+      <c r="D261" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A262" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B262" t="s">
         <v>304</v>
       </c>
-      <c r="C262" s="6" t="s">
+      <c r="C262" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="263" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A263" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B263" s="6" t="s">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A263" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B263" t="s">
         <v>305</v>
       </c>
-      <c r="C263" s="6" t="s">
+      <c r="C263" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="264" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A264" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B264" s="6" t="s">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A264" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B264" t="s">
         <v>306</v>
       </c>
-      <c r="C264" s="6" t="s">
+      <c r="C264" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="265" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A265" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B265" s="6" t="s">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A265" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B265" t="s">
         <v>307</v>
       </c>
-      <c r="C265" s="6" t="s">
+      <c r="C265" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="266" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A266" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B266" s="6" t="s">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A266" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B266" t="s">
         <v>308</v>
       </c>
-      <c r="C266" s="6" t="s">
+      <c r="C266" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="267" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A267" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B267" s="6" t="s">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A267" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B267" t="s">
         <v>309</v>
       </c>
-      <c r="C267" s="6" t="s">
+      <c r="C267" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="268" spans="1:3" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A268" s="6" t="s">
+    <row r="268" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
         <v>9</v>
       </c>
-      <c r="B268" s="6" t="s">
+      <c r="B268" t="s">
         <v>123</v>
       </c>
-      <c r="C268" s="6" t="s">
+      <c r="C268" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="269" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A269" s="6"/>
-      <c r="B269" s="6" t="s">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B269" t="s">
         <v>313</v>
       </c>
-      <c r="C269" s="6" t="s">
+      <c r="C269" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="270" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A270" s="6"/>
-      <c r="B270" s="6" t="s">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B270" t="s">
         <v>314</v>
       </c>
-      <c r="C270" s="6" t="s">
+      <c r="C270" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="271" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A271" s="6"/>
-      <c r="B271" s="6" t="s">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B271" t="s">
         <v>315</v>
       </c>
-      <c r="C271" s="6" t="s">
+      <c r="C271" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="272" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A272" s="6"/>
-      <c r="B272" s="6" t="s">
+    <row r="272" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B272" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C272" s="6" t="s">
+      <c r="C272" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A273" s="6"/>
-      <c r="B273" s="6" t="s">
+      <c r="D272" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="273" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B273" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C273" s="6" t="s">
+      <c r="C273" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A274" s="6"/>
-      <c r="B274" s="6" t="s">
+      <c r="D273" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B274" t="s">
         <v>317</v>
       </c>
-      <c r="C274" s="6" t="s">
+      <c r="C274" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="275" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A275" s="6"/>
-      <c r="B275" s="6" t="s">
+    <row r="275" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B275" t="s">
         <v>318</v>
       </c>
-      <c r="C275" s="6" t="s">
+      <c r="C275" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="276" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A276" s="6"/>
-      <c r="B276" s="6" t="s">
+    <row r="276" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B276" t="s">
         <v>143</v>
       </c>
-      <c r="C276" s="6" t="s">
+      <c r="C276" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="277" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A277" s="6"/>
-      <c r="B277" s="6" t="s">
+    <row r="277" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B277" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C277" s="6" t="s">
+      <c r="C277" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A278" s="6"/>
-      <c r="B278" s="6" t="s">
+      <c r="D277" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B278" t="s">
         <v>58</v>
       </c>
-      <c r="C278" s="6" t="s">
+      <c r="C278" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="279" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A279" s="6"/>
-      <c r="B279" s="6" t="s">
+    <row r="279" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B279" t="s">
         <v>53</v>
       </c>
-      <c r="C279" s="6" t="s">
+      <c r="C279" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="280" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A280" s="6"/>
-      <c r="B280" s="6" t="s">
+    <row r="280" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B280" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C280" s="6" t="s">
+      <c r="C280" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A281" s="6"/>
-      <c r="B281" s="6" t="s">
+      <c r="D280" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="281" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B281" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C281" s="6" t="s">
+      <c r="C281" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A282" s="6"/>
-      <c r="B282" s="6" t="s">
+      <c r="D281" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="282" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B282" t="s">
         <v>56</v>
       </c>
-      <c r="C282" s="6" t="s">
+      <c r="C282" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A283" s="6"/>
-      <c r="B283" s="6" t="s">
+    <row r="283" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B283" t="s">
         <v>196</v>
       </c>
-      <c r="C283" s="6" t="s">
+      <c r="C283" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A284" s="6"/>
-      <c r="B284" s="6" t="s">
+    <row r="284" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B284" t="s">
         <v>59</v>
       </c>
-      <c r="C284" s="6" t="s">
+      <c r="C284" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A285" s="6"/>
-      <c r="B285" s="6" t="s">
+    <row r="285" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B285" t="s">
         <v>103</v>
       </c>
-      <c r="C285" s="6" t="s">
+      <c r="C285" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A286" s="6"/>
-      <c r="B286" s="6" t="s">
+    <row r="286" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B286" t="s">
         <v>321</v>
       </c>
-      <c r="C286" s="6" t="s">
+      <c r="C286" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A287" s="6"/>
-      <c r="B287" s="6" t="s">
+    <row r="287" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B287" t="s">
         <v>323</v>
       </c>
-      <c r="C287" s="6" t="s">
+      <c r="C287" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A288" s="6"/>
-      <c r="B288" s="6" t="s">
+    <row r="288" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B288" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C288" s="6" t="s">
+      <c r="C288" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A289" s="6"/>
-      <c r="B289" s="6" t="s">
+      <c r="D288" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B289" t="s">
         <v>55</v>
       </c>
-      <c r="C289" s="6" t="s">
+      <c r="C289" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A290" s="6"/>
-      <c r="B290" s="6" t="s">
+    <row r="290" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B290" t="s">
         <v>36</v>
       </c>
-      <c r="C290" s="6" t="s">
+      <c r="C290" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A291" s="6"/>
-      <c r="B291" s="6" t="s">
+    <row r="291" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B291" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C291" s="6" t="s">
+      <c r="C291" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A292" s="6"/>
-      <c r="B292" s="6" t="s">
+      <c r="D291" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B292" t="s">
         <v>326</v>
       </c>
-      <c r="C292" s="6" t="s">
+      <c r="C292" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A293" s="6"/>
-      <c r="B293" s="6" t="s">
+    <row r="293" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B293" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C293" s="6" t="s">
+      <c r="C293" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A294" s="6"/>
-      <c r="B294" s="6" t="s">
+      <c r="D293" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B294" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="C294" s="6" t="s">
+      <c r="C294" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A295" s="6"/>
-      <c r="B295" s="6" t="s">
+      <c r="D294" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B295" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="C295" s="6" t="s">
+      <c r="C295" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A296" s="6"/>
-      <c r="B296" s="6" t="s">
+      <c r="D295" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="296" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B296" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C296" s="6" t="s">
+      <c r="C296" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A297" s="6"/>
-      <c r="B297" s="6" t="s">
+      <c r="D296" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="297" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B297" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="C297" s="6" t="s">
+      <c r="C297" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A298" s="6"/>
-      <c r="B298" s="6" t="s">
+      <c r="D297" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="298" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B298" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="C298" s="6" t="s">
+      <c r="C298" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A299" s="6"/>
-      <c r="B299" s="6" t="s">
+      <c r="D298" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B299" t="s">
         <v>334</v>
       </c>
-      <c r="C299" s="6" t="s">
+      <c r="C299" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A300" s="6"/>
-      <c r="B300" s="6" t="s">
+    <row r="300" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B300" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="C300" s="6" t="s">
+      <c r="C300" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A301" s="6"/>
-      <c r="B301" s="6" t="s">
+      <c r="D300" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="301" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B301" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C301" s="6" t="s">
+      <c r="C301" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A302" s="6"/>
-      <c r="B302" s="6" t="s">
+      <c r="D301" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B302" t="s">
         <v>337</v>
       </c>
-      <c r="C302" s="6" t="s">
+      <c r="C302" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A303" s="6"/>
-      <c r="B303" s="6" t="s">
+    <row r="303" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B303" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C303" s="6" t="s">
+      <c r="C303" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A304" s="6"/>
-      <c r="B304" s="6" t="s">
+      <c r="D303" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="304" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B304" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C304" s="6" t="s">
+      <c r="C304" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A305" s="6"/>
-      <c r="B305" s="6" t="s">
+      <c r="D304" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="305" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B305" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C305" s="6" t="s">
+      <c r="C305" s="1" t="s">
         <v>333</v>
       </c>
+      <c r="D305" s="8" t="s">
+        <v>364</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7130,7 +7352,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B113"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B32" sqref="B32:B42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bugfix, continue on CTRL class
</commit_message>
<xml_diff>
--- a/data/source/pedpancan_mapping.xlsx
+++ b/data/source/pedpancan_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ochapman/projects/pedpancan_ecdna/data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E9E500-2344-C94D-A35E-496E15D02AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032A2113-7C3E-824B-AC0D-63C4619E5C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="386">
   <si>
     <t>molecular_subtype</t>
   </si>
@@ -987,63 +987,18 @@
     <t>key</t>
   </si>
   <si>
-    <t>Pediatric Type Diffuse Low grade Glioma</t>
-  </si>
-  <si>
     <t>Diffuse astrocytoma (do we know if MYB- or MYBL1-altered)</t>
   </si>
   <si>
-    <t>mesenchymal soft tissue tumors</t>
-  </si>
-  <si>
-    <t>could classify under histocytic disorders or just eliminate since technically not tumor</t>
-  </si>
-  <si>
     <t>CPT</t>
   </si>
   <si>
-    <t>MB is the more typical abbreviation (Nature hates 2-letter abbreviations. Happy to change it back, but that's the reasoning)</t>
-  </si>
-  <si>
-    <t>Other CNS embryonal tumor</t>
-  </si>
-  <si>
     <t>CNS Lymphoma</t>
   </si>
   <si>
     <t>CNSL</t>
   </si>
   <si>
-    <t>Pancreatitic neuroendocrine tumor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cranial and paraspinal nerve tumors - technically could lump MPNST and NFP in this category as well </t>
-  </si>
-  <si>
-    <t>Circumscribed astrocytoma?</t>
-  </si>
-  <si>
-    <t>Circumscribed astrocytic gliomas</t>
-  </si>
-  <si>
-    <t>Could include within SARC and make spindle cell subtype</t>
-  </si>
-  <si>
-    <t>Could include within SARC and make synovial sarcoma as subtype</t>
-  </si>
-  <si>
-    <t>could classify under sarcoma</t>
-  </si>
-  <si>
-    <t>could classify under sarcoma (anggiomatoid fibrous histiocytoma)</t>
-  </si>
-  <si>
-    <t>MRT is apparently "Rhabdoid Cancer, Kidney" according to SJ</t>
-  </si>
-  <si>
-    <t>Gastric neuroendocrine tumor - could be classified under neuroendocrine tumor</t>
-  </si>
-  <si>
     <t>NET</t>
   </si>
   <si>
@@ -1065,57 +1020,18 @@
     <t>Clear Cell Sarcoma</t>
   </si>
   <si>
-    <t>Clarify what this stands for (Clear Cell Sarcoma)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Carcinoma, NOS)</t>
-  </si>
-  <si>
     <t>MSTT</t>
   </si>
   <si>
-    <t>Carcinoma, NOS</t>
-  </si>
-  <si>
     <t>Choroid Plexus Tumors</t>
   </si>
   <si>
     <t>Chordoma</t>
   </si>
   <si>
-    <t>What does DES stand for? (Desmoid/Aggressive Fibromatosis)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Fibromyxoid Sarcoma)</t>
-  </si>
-  <si>
-    <t>What does BYST stand for? (Yolk Sac Tumor, Brain)</t>
-  </si>
-  <si>
-    <t>Pleomorphic dermal sarcoma? (Dysgerminoma, Pelvis)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Dysgerminoma, Ovarian)</t>
-  </si>
-  <si>
-    <t>What does GNOS stand for (Glioma, NOS)</t>
-  </si>
-  <si>
-    <t>What does HB stand for (Hepatoblastoma)</t>
-  </si>
-  <si>
     <t>Clarify what this stands for (High-Grade Calvarium Sarcoma)</t>
   </si>
   <si>
-    <t>Clarify what this stand for (Inflammatory Myofibroblastic Stomach Tumor)</t>
-  </si>
-  <si>
-    <t>Is this type of malignant rhabdoid tumor (Malignant Rhabdoid Tumor of the Liver)</t>
-  </si>
-  <si>
-    <t>What does MS stand for? (Myeloid Sarcoma)</t>
-  </si>
-  <si>
     <t>Desmoid/Aggressive Fibromatosis</t>
   </si>
   <si>
@@ -1182,12 +1098,6 @@
     <t>Malignant Peripheral Nerve Sheath Tumor</t>
   </si>
   <si>
-    <t>Malignant Rhabdoid Tumor of the Liver</t>
-  </si>
-  <si>
-    <t>Rhabdoid Cancer, Kidney</t>
-  </si>
-  <si>
     <t>Myeloid Sarcoma</t>
   </si>
   <si>
@@ -1212,9 +1122,6 @@
     <t>Pheochromocytoma</t>
   </si>
   <si>
-    <t>perihillar cholangiosarcoma or primary hepatocellular carcinoma - if later, can be under HCC (neither, Pheochromocytoma)</t>
-  </si>
-  <si>
     <t>Pineocytoma</t>
   </si>
   <si>
@@ -1230,9 +1137,6 @@
     <t>Rhabdomyosarcoma</t>
   </si>
   <si>
-    <t>Sarcomas</t>
-  </si>
-  <si>
     <t>Squamous Cell Carcinoma, NOS</t>
   </si>
   <si>
@@ -1263,31 +1167,31 @@
     <t>Wilms Tumor</t>
   </si>
   <si>
-    <t>Clarify what this stands for (Undifferentiated Embryonal Sarcoma of the Liver)</t>
-  </si>
-  <si>
-    <t>What is THPA? (Papillary Thyroid Cancer)</t>
-  </si>
-  <si>
-    <t>Thyroid cancer? (Follicular Thyroid Cancer)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Solid Cancer Unknown Primary)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Spindle Epithelial Tumor with Thymus-Like Differentiation)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Squamous Cell Carcinoma, NOS)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Spindle Cell Sarcoma, NOS)</t>
-  </si>
-  <si>
-    <t>Clarify what this stands for (Round Cell Sarcoma, NOS)</t>
-  </si>
-  <si>
-    <t>What does PINC stand for? (Pineocytoma)</t>
+    <t>Other Sarcomas</t>
+  </si>
+  <si>
+    <t>CARC</t>
+  </si>
+  <si>
+    <t>Other Carcinomas</t>
+  </si>
+  <si>
+    <t>HBL</t>
+  </si>
+  <si>
+    <t>DAST</t>
+  </si>
+  <si>
+    <t>Extracranial Rhabdoid Tumors</t>
+  </si>
+  <si>
+    <t>OST</t>
+  </si>
+  <si>
+    <t>THCA</t>
+  </si>
+  <si>
+    <t>Epilepsy, chronic rasmussen encephalitis</t>
   </si>
 </sst>
 </file>
@@ -1803,18 +1707,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2201,10 +2100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H289"/>
+  <dimension ref="A1:F290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="B283" sqref="B283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2215,7 +2114,7 @@
     <col min="4" max="4" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>312</v>
       </c>
@@ -2235,7 +2134,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>282</v>
       </c>
@@ -2246,7 +2145,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2257,7 +2156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2278,13 +2177,8 @@
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2294,13 +2188,8 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>282</v>
       </c>
@@ -2310,13 +2199,8 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>282</v>
       </c>
@@ -2326,13 +2210,8 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2343,7 +2222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2354,7 +2233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -2365,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2376,7 +2255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -2387,7 +2266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -2398,7 +2277,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -2409,7 +2288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -2420,7 +2299,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2310,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>282</v>
       </c>
@@ -2442,7 +2321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -2453,7 +2332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -2464,7 +2343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>282</v>
       </c>
@@ -2475,7 +2354,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2486,7 +2365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -2497,7 +2376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>282</v>
       </c>
@@ -2508,7 +2387,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>282</v>
       </c>
@@ -2516,13 +2395,14 @@
         <v>303</v>
       </c>
       <c r="C25" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>282</v>
       </c>
@@ -2530,13 +2410,14 @@
         <v>246</v>
       </c>
       <c r="C26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -2547,7 +2428,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -2558,7 +2439,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>282</v>
       </c>
@@ -2569,7 +2450,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>282</v>
       </c>
@@ -2577,13 +2458,14 @@
         <v>242</v>
       </c>
       <c r="C30" t="s">
+        <v>378</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" t="s">
         <v>242</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
@@ -2591,11 +2473,11 @@
         <v>179</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -2647,7 +2529,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2658,7 +2540,7 @@
         <v>22</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2669,7 +2551,7 @@
         <v>32</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2680,7 +2562,7 @@
         <v>29</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -2691,7 +2573,7 @@
         <v>30</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2702,7 +2584,7 @@
         <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2713,7 +2595,7 @@
         <v>34</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2724,11 +2606,9 @@
         <v>240</v>
       </c>
       <c r="C43" t="s">
-        <v>240</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>349</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
@@ -2784,9 +2664,7 @@
       <c r="C48" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>323</v>
-      </c>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -2964,7 +2842,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>6</v>
       </c>
@@ -2975,7 +2853,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>9</v>
       </c>
@@ -2986,7 +2864,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
@@ -2997,7 +2875,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>9</v>
       </c>
@@ -3008,7 +2886,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>282</v>
       </c>
@@ -3019,7 +2897,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>282</v>
       </c>
@@ -3030,7 +2908,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>282</v>
       </c>
@@ -3041,7 +2919,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>282</v>
       </c>
@@ -3052,7 +2930,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>282</v>
       </c>
@@ -3062,11 +2940,9 @@
       <c r="C73" t="s">
         <v>308</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>282</v>
       </c>
@@ -3076,11 +2952,8 @@
       <c r="C74" t="s">
         <v>308</v>
       </c>
-      <c r="D74" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>282</v>
       </c>
@@ -3090,11 +2963,9 @@
       <c r="C75" t="s">
         <v>308</v>
       </c>
-      <c r="D75" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>282</v>
       </c>
@@ -3105,7 +2976,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>282</v>
       </c>
@@ -3116,7 +2987,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>282</v>
       </c>
@@ -3124,13 +2995,13 @@
         <v>211</v>
       </c>
       <c r="C78" t="s">
+        <v>309</v>
+      </c>
+      <c r="E78" t="s">
         <v>211</v>
       </c>
-      <c r="D78" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
@@ -3141,7 +3012,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>9</v>
       </c>
@@ -3328,7 +3199,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>0</v>
       </c>
@@ -3339,7 +3210,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>0</v>
       </c>
@@ -3350,7 +3221,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>282</v>
       </c>
@@ -3361,7 +3232,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>0</v>
       </c>
@@ -3372,7 +3243,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>0</v>
       </c>
@@ -3383,7 +3254,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>0</v>
       </c>
@@ -3394,7 +3265,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -3405,7 +3276,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>0</v>
       </c>
@@ -3416,7 +3287,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>0</v>
       </c>
@@ -3427,7 +3298,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>0</v>
       </c>
@@ -3438,7 +3309,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>0</v>
       </c>
@@ -3449,7 +3320,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>282</v>
       </c>
@@ -3460,7 +3331,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>0</v>
       </c>
@@ -3471,7 +3342,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>0</v>
       </c>
@@ -3482,7 +3353,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>0</v>
       </c>
@@ -3493,7 +3364,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>282</v>
       </c>
@@ -3501,13 +3372,10 @@
         <v>244</v>
       </c>
       <c r="C112" t="s">
-        <v>244</v>
-      </c>
-      <c r="D112" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>282</v>
       </c>
@@ -3518,7 +3386,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>282</v>
       </c>
@@ -3526,13 +3394,16 @@
         <v>215</v>
       </c>
       <c r="C114" t="s">
+        <v>183</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E114" t="s">
         <v>215</v>
       </c>
-      <c r="D114" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>0</v>
       </c>
@@ -3543,7 +3414,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +3425,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>0</v>
       </c>
@@ -3565,7 +3436,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -3576,7 +3447,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>0</v>
       </c>
@@ -3587,7 +3458,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>0</v>
       </c>
@@ -3598,7 +3469,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>0</v>
       </c>
@@ -3609,7 +3480,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>0</v>
       </c>
@@ -3620,7 +3491,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>0</v>
       </c>
@@ -3631,7 +3502,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>0</v>
       </c>
@@ -3642,7 +3513,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>0</v>
       </c>
@@ -3653,7 +3524,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>0</v>
       </c>
@@ -3664,7 +3535,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>0</v>
       </c>
@@ -3675,7 +3546,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>26</v>
       </c>
@@ -3862,7 +3733,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>282</v>
       </c>
@@ -3873,7 +3744,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>282</v>
       </c>
@@ -3884,7 +3755,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>282</v>
       </c>
@@ -3895,7 +3766,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>282</v>
       </c>
@@ -3906,7 +3777,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>282</v>
       </c>
@@ -3917,7 +3788,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>282</v>
       </c>
@@ -3928,7 +3799,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>282</v>
       </c>
@@ -3939,7 +3810,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>282</v>
       </c>
@@ -3950,7 +3821,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>282</v>
       </c>
@@ -3961,7 +3832,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>282</v>
       </c>
@@ -3972,7 +3843,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>282</v>
       </c>
@@ -3983,7 +3854,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>6</v>
       </c>
@@ -3994,7 +3865,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +3876,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>282</v>
       </c>
@@ -4015,85 +3886,70 @@
       <c r="C158" t="s">
         <v>265</v>
       </c>
-      <c r="D158" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>26</v>
       </c>
-      <c r="B159" s="4" t="s">
+      <c r="B159" t="s">
         <v>107</v>
       </c>
-      <c r="C159" s="4" t="s">
+      <c r="C159" t="s">
         <v>105</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D159" s="3"/>
+      <c r="E159" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F159" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="E159" s="4"/>
-      <c r="F159" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="G159" s="4"/>
-      <c r="H159" s="4"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A160" s="6" t="s">
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B160" t="s">
         <v>44</v>
       </c>
-      <c r="C160" s="4" t="s">
+      <c r="C160" t="s">
         <v>105</v>
       </c>
-      <c r="D160" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="E160" s="4"/>
-      <c r="F160" s="4"/>
-      <c r="G160" s="4"/>
-      <c r="H160" s="4"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A161" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="B161" s="4" t="s">
+      <c r="D160" s="3"/>
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B161" t="s">
         <v>214</v>
       </c>
-      <c r="C161" s="4" t="s">
+      <c r="C161" t="s">
         <v>105</v>
       </c>
-      <c r="D161" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="E161" s="4"/>
-      <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
-      <c r="H161" s="4"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A162" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="B162" s="4" t="s">
+      <c r="D161" s="5"/>
+      <c r="E161" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B162" t="s">
         <v>219</v>
       </c>
-      <c r="C162" s="4" t="s">
+      <c r="C162" t="s">
         <v>105</v>
       </c>
-      <c r="D162" s="9" t="s">
-        <v>328</v>
-      </c>
-      <c r="E162" s="4"/>
-      <c r="F162" s="4"/>
-      <c r="G162" s="4"/>
-      <c r="H162" s="4"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D162" s="5"/>
+      <c r="E162" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>0</v>
       </c>
@@ -4104,7 +3960,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>0</v>
       </c>
@@ -4115,7 +3971,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>0</v>
       </c>
@@ -4126,7 +3982,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>0</v>
       </c>
@@ -4137,7 +3993,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>0</v>
       </c>
@@ -4148,7 +4004,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>0</v>
       </c>
@@ -4159,7 +4015,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>0</v>
       </c>
@@ -4170,7 +4026,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>0</v>
       </c>
@@ -4181,7 +4037,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>0</v>
       </c>
@@ -4192,7 +4048,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>0</v>
       </c>
@@ -4203,7 +4059,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>0</v>
       </c>
@@ -4214,7 +4070,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>0</v>
       </c>
@@ -4225,7 +4081,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>0</v>
       </c>
@@ -4236,7 +4092,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>0</v>
       </c>
@@ -4442,11 +4298,9 @@
         <v>276</v>
       </c>
       <c r="C194" t="s">
-        <v>142</v>
-      </c>
-      <c r="D194" s="9" t="s">
-        <v>322</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="D194" s="5"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
@@ -4456,7 +4310,7 @@
         <v>277</v>
       </c>
       <c r="C195" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -4467,7 +4321,7 @@
         <v>278</v>
       </c>
       <c r="C196" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -4478,7 +4332,7 @@
         <v>279</v>
       </c>
       <c r="C197" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -4489,7 +4343,7 @@
         <v>280</v>
       </c>
       <c r="C198" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -4500,7 +4354,7 @@
         <v>281</v>
       </c>
       <c r="C199" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -4511,7 +4365,7 @@
         <v>141</v>
       </c>
       <c r="C200" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -4522,7 +4376,7 @@
         <v>143</v>
       </c>
       <c r="C201" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -4533,7 +4387,7 @@
         <v>144</v>
       </c>
       <c r="C202" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -4544,7 +4398,7 @@
         <v>145</v>
       </c>
       <c r="C203" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -4555,7 +4409,7 @@
         <v>146</v>
       </c>
       <c r="C204" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -4566,7 +4420,7 @@
         <v>176</v>
       </c>
       <c r="C205" t="s">
-        <v>142</v>
+        <v>280</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -4755,9 +4609,6 @@
       <c r="C222" t="s">
         <v>266</v>
       </c>
-      <c r="D222" t="s">
-        <v>334</v>
-      </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
@@ -4767,11 +4618,9 @@
         <v>271</v>
       </c>
       <c r="C223" t="s">
-        <v>271</v>
-      </c>
-      <c r="D223" s="3" t="s">
-        <v>358</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="D223" s="3"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
@@ -4781,11 +4630,9 @@
         <v>300</v>
       </c>
       <c r="C224" t="s">
-        <v>300</v>
-      </c>
-      <c r="D224" s="3" t="s">
-        <v>359</v>
-      </c>
+        <v>198</v>
+      </c>
+      <c r="D224" s="3"/>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
@@ -4806,11 +4653,9 @@
         <v>293</v>
       </c>
       <c r="C226" t="s">
-        <v>345</v>
-      </c>
-      <c r="D226" s="8" t="s">
-        <v>319</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="D226" s="4"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
@@ -4820,10 +4665,7 @@
         <v>196</v>
       </c>
       <c r="C227" t="s">
-        <v>345</v>
-      </c>
-      <c r="D227" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
@@ -4922,11 +4764,9 @@
         <v>272</v>
       </c>
       <c r="C236" t="s">
-        <v>336</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>335</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="D236" s="3"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
@@ -4936,11 +4776,9 @@
         <v>270</v>
       </c>
       <c r="C237" t="s">
-        <v>336</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>326</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="D237" s="3"/>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
@@ -4975,7 +4813,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>9</v>
       </c>
@@ -4986,7 +4824,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>9</v>
       </c>
@@ -4997,7 +4835,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>9</v>
       </c>
@@ -5008,7 +4846,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>9</v>
       </c>
@@ -5018,11 +4856,8 @@
       <c r="C244" t="s">
         <v>314</v>
       </c>
-      <c r="D244" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>9</v>
       </c>
@@ -5033,7 +4868,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>9</v>
       </c>
@@ -5043,11 +4878,8 @@
       <c r="C246" t="s">
         <v>314</v>
       </c>
-      <c r="D246" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>9</v>
       </c>
@@ -5058,7 +4890,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>9</v>
       </c>
@@ -5069,7 +4901,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>9</v>
       </c>
@@ -5077,13 +4909,12 @@
         <v>173</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D249" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="D249" s="1"/>
+      <c r="E249" s="1"/>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
         <v>282</v>
       </c>
@@ -5091,10 +4922,10 @@
         <v>191</v>
       </c>
       <c r="C250" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
         <v>282</v>
       </c>
@@ -5102,10 +4933,10 @@
         <v>233</v>
       </c>
       <c r="C251" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>6</v>
       </c>
@@ -5116,7 +4947,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>9</v>
       </c>
@@ -5127,7 +4958,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>6</v>
       </c>
@@ -5138,7 +4969,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
         <v>282</v>
       </c>
@@ -5149,7 +4980,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
         <v>282</v>
       </c>
@@ -5157,11 +4988,9 @@
         <v>273</v>
       </c>
       <c r="C256" t="s">
-        <v>273</v>
-      </c>
-      <c r="D256" s="3" t="s">
-        <v>392</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="D256" s="3"/>
     </row>
     <row r="257" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
@@ -5171,10 +5000,7 @@
         <v>217</v>
       </c>
       <c r="C257" t="s">
-        <v>217</v>
-      </c>
-      <c r="D257" t="s">
-        <v>417</v>
+        <v>8</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
@@ -5185,10 +5011,7 @@
         <v>291</v>
       </c>
       <c r="C258" t="s">
-        <v>292</v>
-      </c>
-      <c r="D258" t="s">
-        <v>327</v>
+        <v>8</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
@@ -5199,7 +5022,7 @@
         <v>234</v>
       </c>
       <c r="C259" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
@@ -5232,10 +5055,11 @@
         <v>254</v>
       </c>
       <c r="C262" t="s">
+        <v>183</v>
+      </c>
+      <c r="D262" s="3"/>
+      <c r="E262" t="s">
         <v>254</v>
-      </c>
-      <c r="D262" s="3" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
@@ -5314,9 +5138,6 @@
       <c r="C269" t="s">
         <v>183</v>
       </c>
-      <c r="D269" t="s">
-        <v>333</v>
-      </c>
       <c r="E269" t="s">
         <v>262</v>
       </c>
@@ -5345,9 +5166,6 @@
       <c r="C271" t="s">
         <v>183</v>
       </c>
-      <c r="D271" t="s">
-        <v>332</v>
-      </c>
       <c r="E271" t="s">
         <v>257</v>
       </c>
@@ -5362,9 +5180,7 @@
       <c r="C272" t="s">
         <v>183</v>
       </c>
-      <c r="D272" s="1" t="s">
-        <v>350</v>
-      </c>
+      <c r="D272" s="1"/>
       <c r="E272" t="s">
         <v>248</v>
       </c>
@@ -5390,10 +5206,8 @@
       <c r="C274" t="s">
         <v>183</v>
       </c>
-      <c r="D274" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="E274" s="10" t="s">
+      <c r="D274" s="4"/>
+      <c r="E274" t="s">
         <v>288</v>
       </c>
     </row>
@@ -5407,10 +5221,8 @@
       <c r="C275" t="s">
         <v>183</v>
       </c>
-      <c r="D275" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="E275" s="10" t="s">
+      <c r="D275" s="4"/>
+      <c r="E275" t="s">
         <v>238</v>
       </c>
     </row>
@@ -5422,10 +5234,10 @@
         <v>247</v>
       </c>
       <c r="C276" t="s">
+        <v>378</v>
+      </c>
+      <c r="E276" t="s">
         <v>247</v>
-      </c>
-      <c r="D276" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
@@ -5436,10 +5248,11 @@
         <v>78</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D277" s="8" t="s">
-        <v>327</v>
+        <v>8</v>
+      </c>
+      <c r="D277" s="4"/>
+      <c r="E277" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.2">
@@ -5450,10 +5263,11 @@
         <v>184</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D278" s="8" t="s">
-        <v>327</v>
+        <v>8</v>
+      </c>
+      <c r="D278" s="4"/>
+      <c r="E278" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
@@ -5464,10 +5278,11 @@
         <v>243</v>
       </c>
       <c r="C279" t="s">
-        <v>243</v>
-      </c>
-      <c r="D279" s="3" t="s">
-        <v>415</v>
+        <v>183</v>
+      </c>
+      <c r="D279" s="3"/>
+      <c r="E279" s="1" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.2">
@@ -5510,11 +5325,12 @@
       <c r="B283" t="s">
         <v>255</v>
       </c>
-      <c r="C283" t="s">
+      <c r="C283" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D283" s="1"/>
+      <c r="E283" t="s">
         <v>255</v>
-      </c>
-      <c r="D283" s="1" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
@@ -5527,9 +5343,7 @@
       <c r="C284" t="s">
         <v>197</v>
       </c>
-      <c r="D284" s="1" t="s">
-        <v>412</v>
-      </c>
+      <c r="D284" s="1"/>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
@@ -5538,11 +5352,12 @@
       <c r="B285" t="s">
         <v>269</v>
       </c>
-      <c r="C285" t="s">
+      <c r="C285" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D285" s="3"/>
+      <c r="E285" t="s">
         <v>269</v>
-      </c>
-      <c r="D285" s="3" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.2">
@@ -5553,10 +5368,10 @@
         <v>241</v>
       </c>
       <c r="C286" t="s">
+        <v>384</v>
+      </c>
+      <c r="E286" t="s">
         <v>241</v>
-      </c>
-      <c r="D286" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
@@ -5567,10 +5382,10 @@
         <v>253</v>
       </c>
       <c r="C287" t="s">
+        <v>183</v>
+      </c>
+      <c r="E287" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D287" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
@@ -5593,6 +5408,17 @@
       </c>
       <c r="C289" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A290" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B290" t="s">
+        <v>385</v>
+      </c>
+      <c r="C290" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5600,7 +5426,7 @@
     <sortCondition ref="C2:C289"/>
   </sortState>
   <phoneticPr fontId="19" type="noConversion"/>
-  <conditionalFormatting sqref="A1:E32 A34:E77 A33:C33 E33 A125:E165 A124:C124 E124 A78:C78 E78 A79:E123 A232:C232 E232 A166:C166 E166 A167:E231 A233:E281 A284:E1048576 A282:C283 E282:E283">
+  <conditionalFormatting sqref="A1:E32 A33:C33 E33 A34:E77 A78:C78 E78 A79:E123 A124:C124 E124 A125:E165 A166:C166 E166 A232:C232 E232 A167:E231 A233:E278 A287:D287 A280:E281 A279:D279 E282:E283 A282:C283 A284:E286 A288:E1048576">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>"NOT(ISBLANK)"</formula>
     </cfRule>
@@ -5611,10 +5437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92187E74-4F7E-DD4F-A405-6C0E523CB693}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5632,7 +5458,7 @@
         <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5640,7 +5466,7 @@
         <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -5648,7 +5474,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5656,7 +5482,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -5664,7 +5490,7 @@
         <v>309</v>
       </c>
       <c r="B6" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -5672,23 +5498,23 @@
         <v>303</v>
       </c>
       <c r="B7" t="s">
-        <v>342</v>
+        <v>327</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>378</v>
       </c>
       <c r="B8" t="s">
-        <v>346</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B9" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5701,10 +5527,10 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B11" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5712,7 +5538,7 @@
         <v>249</v>
       </c>
       <c r="B12" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5720,7 +5546,7 @@
         <v>240</v>
       </c>
       <c r="B13" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5728,7 +5554,7 @@
         <v>194</v>
       </c>
       <c r="B14" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -5736,7 +5562,7 @@
         <v>206</v>
       </c>
       <c r="B15" t="s">
-        <v>362</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -5744,7 +5570,7 @@
         <v>289</v>
       </c>
       <c r="B16" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -5752,7 +5578,7 @@
         <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>364</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -5760,15 +5586,15 @@
         <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>365</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="B19" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -5776,7 +5602,7 @@
         <v>248</v>
       </c>
       <c r="B20" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -5784,7 +5610,7 @@
         <v>308</v>
       </c>
       <c r="B21" t="s">
-        <v>368</v>
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -5792,7 +5618,7 @@
         <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -5800,7 +5626,7 @@
         <v>211</v>
       </c>
       <c r="B23" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -5808,7 +5634,7 @@
         <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>371</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -5816,7 +5642,7 @@
         <v>244</v>
       </c>
       <c r="B25" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -5824,7 +5650,7 @@
         <v>260</v>
       </c>
       <c r="B26" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -5832,7 +5658,7 @@
         <v>215</v>
       </c>
       <c r="B27" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -5840,7 +5666,7 @@
         <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -5848,7 +5674,7 @@
         <v>198</v>
       </c>
       <c r="B29" t="s">
-        <v>376</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -5864,15 +5690,15 @@
         <v>265</v>
       </c>
       <c r="B31" t="s">
-        <v>377</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
+      <c r="A32" t="s">
         <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>378</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -5880,7 +5706,7 @@
         <v>142</v>
       </c>
       <c r="B33" t="s">
-        <v>379</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -5888,7 +5714,7 @@
         <v>190</v>
       </c>
       <c r="B34" t="s">
-        <v>380</v>
+        <v>352</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -5904,7 +5730,7 @@
         <v>158</v>
       </c>
       <c r="B36" t="s">
-        <v>381</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -5912,267 +5738,259 @@
         <v>266</v>
       </c>
       <c r="B37" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>271</v>
+        <v>300</v>
       </c>
       <c r="B38" t="s">
-        <v>382</v>
+        <v>354</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>300</v>
+      <c r="A39" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="B39" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>162</v>
+      <c r="A40" t="s">
+        <v>268</v>
       </c>
       <c r="B40" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>268</v>
+      <c r="A41" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B41" t="s">
-        <v>386</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>164</v>
+      <c r="A42" t="s">
+        <v>321</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>357</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>336</v>
+      <c r="A43" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B43" t="s">
-        <v>387</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>171</v>
+        <v>314</v>
       </c>
       <c r="B44" t="s">
-        <v>170</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>314</v>
+        <v>174</v>
       </c>
       <c r="B45" t="s">
-        <v>388</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>174</v>
+      <c r="A46" t="s">
+        <v>191</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
       <c r="B47" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>270</v>
+      <c r="A48" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="B48" t="s">
-        <v>390</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>209</v>
+      <c r="A49" t="s">
+        <v>273</v>
       </c>
       <c r="B49" t="s">
-        <v>177</v>
+        <v>361</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>273</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
-        <v>391</v>
+        <v>362</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>217</v>
+        <v>292</v>
       </c>
       <c r="B51" t="s">
-        <v>393</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>292</v>
+        <v>192</v>
       </c>
       <c r="B52" t="s">
-        <v>291</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="B53" t="s">
-        <v>394</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>201</v>
+        <v>254</v>
       </c>
       <c r="B54" t="s">
-        <v>395</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>254</v>
+      <c r="A55" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="B55" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>181</v>
+      <c r="A56" t="s">
+        <v>183</v>
       </c>
       <c r="B56" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>183</v>
+        <v>247</v>
       </c>
       <c r="B57" t="s">
-        <v>398</v>
+        <v>367</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>247</v>
+      <c r="A58" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>399</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>79</v>
+      <c r="A59" t="s">
+        <v>243</v>
       </c>
       <c r="B59" t="s">
-        <v>184</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>243</v>
+      <c r="A60" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B60" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>186</v>
+      <c r="A61" t="s">
+        <v>255</v>
       </c>
       <c r="B61" t="s">
-        <v>401</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>255</v>
+        <v>197</v>
       </c>
       <c r="B62" t="s">
-        <v>402</v>
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>197</v>
+        <v>238</v>
       </c>
       <c r="B63" t="s">
-        <v>403</v>
+        <v>372</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>238</v>
+        <v>269</v>
       </c>
       <c r="B64" t="s">
-        <v>404</v>
+        <v>373</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="B65" t="s">
-        <v>405</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="B66" t="s">
-        <v>406</v>
+        <v>375</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>253</v>
+        <v>199</v>
       </c>
       <c r="B67" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>199</v>
-      </c>
-      <c r="B68" t="s">
-        <v>408</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A288">
-    <sortCondition ref="A2:A288"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A287">
+    <sortCondition ref="A2:A287"/>
   </sortState>
-  <conditionalFormatting sqref="A290:A1048576 A1:A69">
+  <conditionalFormatting sqref="A289:A1048576 A1:A68">
     <cfRule type="expression" dxfId="1" priority="3">
       <formula>"NOT(ISBLANK)"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B52:B53">
+  <conditionalFormatting sqref="B51:B52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"NOT(ISBLANK)"</formula>
     </cfRule>

</xml_diff>